<commit_message>
finished new xlsx parser
</commit_message>
<xml_diff>
--- a/files/success-file-example.xlsx
+++ b/files/success-file-example.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24617"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74E800DB-FEFA-4B35-853F-753BFEB0634A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61E3042E-2399-47E1-BA2E-9E40A38E843D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,13 +28,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Country name</t>
-  </si>
-  <si>
-    <t>ID</t>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Country Name</t>
+  </si>
+  <si>
+    <t>AMPLYFI_NBR</t>
   </si>
   <si>
     <t>STRABAG SE VAT AT</t>
@@ -469,7 +469,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>